<commit_message>
nmf: pre-final optimization, excel-optim introduced, comparison of cases
</commit_message>
<xml_diff>
--- a/Project_python/out/NMF/topics_map.xlsx
+++ b/Project_python/out/NMF/topics_map.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:1.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.523|x10:0.000|x11:0.477|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:1.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:1.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:1.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:1.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:1.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.164|x4:0.000|x5:0.000|x6:0.836|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.634|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.366|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:1.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:1.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:1.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:1.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:1.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:1.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:1.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>x1:0.848|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.152|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:1.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:1.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.784|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.216|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:1.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:1.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:1.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:1.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:1.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:1.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:1.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.760|x10:0.240|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:1.000|x17:0.000</t>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.211|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.789|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:1.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+          <t>x1:0.000|x2:1.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,57 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>x1:0.000|x2:0.000|x3:0.652|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.348|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:1.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.143|x12:0.857|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>x1:0.000|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:1.000|x17:0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>x1:0.000|x2:0.000|x3:1.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.000|x12:0.000|x13:0.000|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>x1:0.391|x2:0.000|x3:0.000|x4:0.000|x5:0.000|x6:0.000|x7:0.000|x8:0.000|x9:0.000|x10:0.000|x11:0.266|x12:0.000|x13:0.343|x14:0.000|x15:0.000|x16:0.000|x17:0.000</t>
         </is>
       </c>
     </row>

</xml_diff>